<commit_message>
EPBDS-11585 RulesType annotation must look for SPR custom type classes, added ability to deserialize JSON/XML in ObjectSerializer
</commit_message>
<xml_diff>
--- a/ITEST/itest.storelogdata/openl-repository/deployments/deployment6/simple6/Main.xlsx
+++ b/ITEST/itest.storelogdata/openl-repository/deployments/deployment6/simple6/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService-WADL-WSDL\openl-repository\deployments\simple1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\ITEST\itest.storelogdata\openl-repository\deployments\deployment6\simple6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020D7861-BB04-4B62-ACDC-87F6E6C194CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72717E-F36D-4F96-8179-5CE14C66396C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="90" windowWidth="31815" windowHeight="20565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Rule</t>
   </si>
@@ -292,6 +292,27 @@
   </si>
   <si>
     <t>Value2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult DoSomething()</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Foo1</t>
+  </si>
+  <si>
+    <t>Foo2</t>
+  </si>
+  <si>
+    <t>= test ($Foo1)</t>
+  </si>
+  <si>
+    <t>= 11</t>
   </si>
 </sst>
 </file>
@@ -598,38 +619,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,226 +1023,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E21"/>
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="17">
         <v>0</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="18">
         <v>11</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="21">
         <v>12</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <v>17</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="21">
         <v>18</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="22">
         <v>21</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="25">
         <v>22</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="26">
         <v>23</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="17">
         <v>0</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="18">
         <v>11</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="21">
         <v>12</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="22">
         <v>17</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="21">
         <v>18</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="22">
         <v>21</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="25">
         <v>22</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="26">
         <v>23</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="27" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
EPBDS-11585 RulesType annotation must look for SPR custom type classes, added ability to deserialize JSON/XML in ObjectSerializer (#98)
</commit_message>
<xml_diff>
--- a/ITEST/itest.storelogdata/openl-repository/deployments/deployment6/simple6/Main.xlsx
+++ b/ITEST/itest.storelogdata/openl-repository/deployments/deployment6/simple6/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService-WADL-WSDL\openl-repository\deployments\simple1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\ITEST\itest.storelogdata\openl-repository\deployments\deployment6\simple6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020D7861-BB04-4B62-ACDC-87F6E6C194CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72717E-F36D-4F96-8179-5CE14C66396C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="90" windowWidth="31815" windowHeight="20565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Rule</t>
   </si>
@@ -292,6 +292,27 @@
   </si>
   <si>
     <t>Value2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult DoSomething()</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Foo1</t>
+  </si>
+  <si>
+    <t>Foo2</t>
+  </si>
+  <si>
+    <t>= test ($Foo1)</t>
+  </si>
+  <si>
+    <t>= 11</t>
   </si>
 </sst>
 </file>
@@ -598,38 +619,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,226 +1023,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E21"/>
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="17">
         <v>0</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="18">
         <v>11</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="21">
         <v>12</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <v>17</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="21">
         <v>18</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="22">
         <v>21</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="25">
         <v>22</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="26">
         <v>23</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="17">
         <v>0</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="18">
         <v>11</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="21">
         <v>12</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="22">
         <v>17</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="21">
         <v>18</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="22">
         <v>21</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="25">
         <v>22</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="26">
         <v>23</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="27" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>